<commit_message>
error msg for db insert or partition
</commit_message>
<xml_diff>
--- a/Router ip list with 37 SMS numbers.xlsx
+++ b/Router ip list with 37 SMS numbers.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Echo\Echo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Echo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$D$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$103</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -1348,13 +1348,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1659,272 +1659,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="21" customFormat="1">
-      <c r="A1" s="22" t="s">
-        <v>292</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="26" customFormat="1">
-      <c r="A2" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="E2" s="26">
-        <v>1917300427</v>
-      </c>
-      <c r="F2" s="26">
-        <v>1571797880</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="26" customFormat="1">
-      <c r="A3" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="26">
-        <v>1917300427</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="26" customFormat="1">
-      <c r="A4" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="E4" s="26">
-        <v>1917300427</v>
-      </c>
-      <c r="F4" s="26">
-        <v>1571797880</v>
-      </c>
-      <c r="G4" s="26">
-        <v>545454545</v>
-      </c>
-      <c r="H4" s="40">
-        <v>656565</v>
-      </c>
-      <c r="I4" s="40">
-        <v>6565656</v>
-      </c>
-      <c r="J4" s="40">
-        <v>5656565</v>
-      </c>
-      <c r="K4" s="40">
-        <v>5656565</v>
-      </c>
-      <c r="L4" s="40">
-        <v>56565656</v>
-      </c>
-      <c r="M4" s="40">
-        <v>565656565</v>
-      </c>
-      <c r="N4" s="40">
-        <v>4654445</v>
-      </c>
-      <c r="O4" s="40">
-        <v>6565655</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="26">
-        <v>1917300427</v>
-      </c>
-      <c r="F5" s="26">
-        <v>1571797880</v>
-      </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="E6" s="26">
-        <v>1917300427</v>
-      </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" s="26">
-        <v>1917300427</v>
-      </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" s="26">
-        <v>1917300427</v>
-      </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" s="26">
-        <v>1917300427</v>
-      </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="E10" s="26">
-        <v>1571797880</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>248</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" s="26">
-        <v>1571797880</v>
-      </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1954,12 +1693,12 @@
       <c r="D1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="39" t="s">
         <v>347</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:11" s="26" customFormat="1">
       <c r="A2" s="12" t="s">
@@ -1974,8 +1713,17 @@
       <c r="D2" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="10">
+        <v>1550151309</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1550151433</v>
+      </c>
+      <c r="G2" s="10">
         <v>1917300427</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1550151313</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="26" customFormat="1">
@@ -1991,11 +1739,17 @@
       <c r="D3" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="10">
+        <v>1550151309</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1550151433</v>
+      </c>
+      <c r="G3" s="10">
         <v>1917300427</v>
       </c>
-      <c r="F3" s="26">
-        <v>1571797880</v>
+      <c r="H3" s="10">
+        <v>1550151313</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="26" customFormat="1">
@@ -2011,11 +1765,17 @@
       <c r="D4" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="E4" s="26">
-        <v>14214</v>
-      </c>
-      <c r="F4" s="26">
-        <v>15332</v>
+      <c r="E4" s="10">
+        <v>1550151309</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1550151433</v>
+      </c>
+      <c r="G4" s="10">
+        <v>1551051450</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1550151313</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2031,14 +1791,18 @@
       <c r="D5" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="26">
-        <v>14214</v>
-      </c>
-      <c r="F5" s="26">
-        <v>15332</v>
-      </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="2"/>
+      <c r="E5" s="10">
+        <v>1550151309</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1550151433</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1551051450</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1915334455</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
@@ -2055,13 +1819,18 @@
       <c r="D6" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="26">
-        <v>14214</v>
-      </c>
-      <c r="F6" s="26">
-        <v>15332</v>
-      </c>
-      <c r="G6" s="26"/>
+      <c r="E6" s="10">
+        <v>1550151309</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1550151433</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1551051450</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1915334455</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="12" t="s">
@@ -2076,13 +1845,18 @@
       <c r="D7" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="E7" s="26">
-        <v>14214</v>
-      </c>
-      <c r="F7" s="26">
-        <v>15332</v>
-      </c>
-      <c r="G7" s="26"/>
+      <c r="E7" s="10">
+        <v>1550151309</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1550151433</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1551051450</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1915334455</v>
+      </c>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11">
@@ -2098,13 +1872,16 @@
       <c r="D8" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="26">
-        <v>14214</v>
-      </c>
-      <c r="F8" s="26">
-        <v>15332</v>
-      </c>
-      <c r="G8" s="26"/>
+      <c r="E8" s="10">
+        <v>1551051450</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1571797880</v>
+      </c>
+      <c r="G8" s="10">
+        <v>1551051450</v>
+      </c>
+      <c r="H8" s="10"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11">
@@ -2120,13 +1897,16 @@
       <c r="D9" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E9" s="26">
-        <v>14214</v>
-      </c>
-      <c r="F9" s="26">
-        <v>15332</v>
-      </c>
-      <c r="G9" s="26"/>
+      <c r="E9" s="10">
+        <v>1551051450</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1571797880</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1917300427</v>
+      </c>
+      <c r="H9" s="10"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11">
@@ -2142,11 +1922,16 @@
       <c r="D10" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="10">
+        <v>1551051450</v>
+      </c>
+      <c r="F10" s="10">
         <v>1571797880</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
+      <c r="G10" s="10">
+        <v>1917300427</v>
+      </c>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="12" t="s">
@@ -2161,11 +1946,16 @@
       <c r="D11" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="10">
+        <v>1551051450</v>
+      </c>
+      <c r="F11" s="10">
         <v>1571797880</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="G11" s="10">
+        <v>1917300427</v>
+      </c>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
@@ -2180,13 +1970,16 @@
       <c r="D12" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="26">
-        <v>14214</v>
-      </c>
-      <c r="F12" s="26">
-        <v>546456456</v>
-      </c>
-      <c r="G12" s="26"/>
+      <c r="E12" s="10">
+        <v>1551051450</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1571797880</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1917300427</v>
+      </c>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="12" t="s">
@@ -4154,7 +3947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2"/>
   <sheetViews>
@@ -4171,6 +3964,267 @@
       <c r="A2">
         <v>1917300427</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="21" customFormat="1">
+      <c r="A1" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="26" customFormat="1">
+      <c r="A2" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="E2" s="26">
+        <v>1917300427</v>
+      </c>
+      <c r="F2" s="26">
+        <v>1571797880</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="26" customFormat="1">
+      <c r="A3" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="26">
+        <v>1917300427</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="26" customFormat="1">
+      <c r="A4" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="E4" s="26">
+        <v>1917300427</v>
+      </c>
+      <c r="F4" s="26">
+        <v>1571797880</v>
+      </c>
+      <c r="G4" s="26">
+        <v>545454545</v>
+      </c>
+      <c r="H4" s="38">
+        <v>656565</v>
+      </c>
+      <c r="I4" s="38">
+        <v>6565656</v>
+      </c>
+      <c r="J4" s="38">
+        <v>5656565</v>
+      </c>
+      <c r="K4" s="38">
+        <v>5656565</v>
+      </c>
+      <c r="L4" s="38">
+        <v>56565656</v>
+      </c>
+      <c r="M4" s="38">
+        <v>565656565</v>
+      </c>
+      <c r="N4" s="38">
+        <v>4654445</v>
+      </c>
+      <c r="O4" s="38">
+        <v>6565655</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="26">
+        <v>1917300427</v>
+      </c>
+      <c r="F5" s="26">
+        <v>1571797880</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6" s="26">
+        <v>1917300427</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" s="26">
+        <v>1917300427</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="26">
+        <v>1917300427</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="26">
+        <v>1917300427</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="26">
+        <v>1571797880</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="26">
+        <v>1571797880</v>
+      </c>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>